<commit_message>
Worked on layout, re-routing and BOM.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/itsy_bitsy_mx_shield_v0p1/BOM_FULL.xlsx
+++ b/hardware/pcbs/itsy_bitsy_mx_shield_v0p1/BOM_FULL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
   <si>
     <t xml:space="preserve">JLCPCB</t>
   </si>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">4.7uF ceramic capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C5</t>
+    <t xml:space="preserve">C5</t>
   </si>
   <si>
     <t xml:space="preserve">C19666 </t>
@@ -306,18 +306,6 @@
   </si>
   <si>
     <t xml:space="preserve">C6961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REF3330AIDBZR Voltage References 3V ±0.15%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C140329</t>
   </si>
   <si>
     <t xml:space="preserve">OP07CDR Precision Operational Amplifier</t>
@@ -433,6 +421,15 @@
   </si>
   <si>
     <t xml:space="preserve">811-2679-5-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-Pos. Term. Block, 3.5mm, Vert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1, P2, P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED2635-ND</t>
   </si>
 </sst>
 </file>
@@ -703,13 +700,13 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.78"/>
@@ -903,136 +900,116 @@
       </c>
     </row>
     <row r="13" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="9" t="n">
-        <v>603</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="9" t="n">
-        <v>7</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="9" t="n">
-        <v>603</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="9" t="n">
-        <v>9</v>
-      </c>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E15" s="9" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C16" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E16" s="9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E17" s="9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C18" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E18" s="9" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C19" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E19" s="9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C20" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E20" s="9" t="n">
         <v>1</v>
@@ -1040,16 +1017,16 @@
     </row>
     <row r="21" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C21" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>1</v>
@@ -1057,50 +1034,50 @@
     </row>
     <row r="22" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C22" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E22" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E23" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E24" s="9" t="n">
         <v>2</v>
@@ -1108,195 +1085,175 @@
     </row>
     <row r="25" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C25" s="9" t="n">
+        <v>603</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E25" s="9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="C26" s="9" t="n">
+        <v>603</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E26" s="9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="9" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="34" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" s="9" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="37" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E37" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="E38" s="9" t="n">
         <v>1</v>
@@ -1304,25 +1261,87 @@
     </row>
     <row r="39" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="C43" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added gerber files for rodeostat mx V0.1 R3. Added fab files.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/itsy_bitsy_mx_shield_v0p1/BOM_FULL.xlsx
+++ b/hardware/pcbs/itsy_bitsy_mx_shield_v0p1/BOM_FULL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="114">
   <si>
     <t xml:space="preserve">JLCPCB</t>
   </si>
@@ -167,51 +167,51 @@
     <t xml:space="preserve">C609810 </t>
   </si>
   <si>
-    <t xml:space="preserve">12k Resistor,  1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1,R2,R26,R28,R34,R36,R33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C22790 </t>
+    <t xml:space="preserve">33k Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1,R2,R26,R28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4216</t>
   </si>
   <si>
     <t xml:space="preserve">20k Resistor, 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R3,R5,R6,R8,R10,R13,R23,R25,R29</t>
+    <t xml:space="preserve">R3,R4,R5,R8,R10,R13,R23,R25</t>
   </si>
   <si>
     <t xml:space="preserve">C4184 </t>
   </si>
   <si>
+    <t xml:space="preserve">10k Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6,R7,R9,R18,R19,R24,R33,R34,R36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.9k Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11,R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23184</t>
+  </si>
+  <si>
     <t xml:space="preserve">100k Resistor, 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R4,R12,R20,R21</t>
+    <t xml:space="preserve">R12,R20,R21</t>
   </si>
   <si>
     <t xml:space="preserve">C25803</t>
   </si>
   <si>
-    <t xml:space="preserve">10k Resistor, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7,R9,R18,R19,R24,R27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25804</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.9k Resistor, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11,R22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23184</t>
-  </si>
-  <si>
     <t xml:space="preserve">300k Resistor, 1%</t>
   </si>
   <si>
@@ -246,6 +246,24 @@
   </si>
   <si>
     <t xml:space="preserve">C23025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2k Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C22975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11k Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C103227</t>
   </si>
   <si>
     <t xml:space="preserve">1k Resistor, 1%</t>
@@ -700,7 +718,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="28:28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,133 +918,153 @@
       </c>
     </row>
     <row r="13" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="9" t="n">
+        <v>603</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="9" t="n">
+        <v>603</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E15" s="9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C16" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E16" s="9" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E17" s="9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C18" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E18" s="9" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C19" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E19" s="9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C20" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E20" s="9" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C21" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>1</v>
@@ -1034,16 +1072,16 @@
     </row>
     <row r="22" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C22" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E22" s="9" t="n">
         <v>1</v>
@@ -1051,16 +1089,16 @@
     </row>
     <row r="23" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E23" s="9" t="n">
         <v>1</v>
@@ -1068,16 +1106,16 @@
     </row>
     <row r="24" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E24" s="9" t="n">
         <v>2</v>
@@ -1085,16 +1123,16 @@
     </row>
     <row r="25" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E25" s="9" t="n">
         <v>2</v>
@@ -1102,246 +1140,234 @@
     </row>
     <row r="26" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C26" s="9" t="n">
         <v>603</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E26" s="9" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="27" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="A27" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
+      <c r="A28" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E29" s="9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E30" s="9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="9" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>5</v>
+    <row r="35" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E37" s="9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E38" s="9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>88</v>
-      </c>
       <c r="D39" s="9" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="E39" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E40" s="9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E42" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>